<commit_message>
added assertion in ShoppingCartProductDetailsTest.java
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdatainfo.xlsx
+++ b/src/test/resources/testdata/testdatainfo.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashwi\eclipse-workspace\AutomationFrameworkOpenCart\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3B4AD0-3FF9-474C-B416-C2BBD9B5D62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0AC0BD-AEAD-46F5-9AAB-1EC8A6E3985F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{B8B23BD0-2100-492A-ADF4-82F66140FD90}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{B8B23BD0-2100-492A-ADF4-82F66140FD90}"/>
   </bookViews>
   <sheets>
-    <sheet name="register" sheetId="1" r:id="rId1"/>
-    <sheet name="products" sheetId="2" r:id="rId2"/>
-    <sheet name="productinfo" sheetId="3" r:id="rId3"/>
-    <sheet name="productreview" sheetId="4" r:id="rId4"/>
-    <sheet name="shoppingcartdata" sheetId="5" r:id="rId5"/>
+    <sheet name="products" sheetId="2" r:id="rId1"/>
+    <sheet name="productinfo" sheetId="3" r:id="rId2"/>
+    <sheet name="productreview" sheetId="4" r:id="rId3"/>
+    <sheet name="shoppingcartdata" sheetId="5" r:id="rId4"/>
+    <sheet name="registerationdata" sheetId="1" r:id="rId5"/>
+    <sheet name="registrationdatawithemail" sheetId="6" r:id="rId6"/>
+    <sheet name="negativelogintestdata" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="89">
   <si>
     <t>firstname</t>
   </si>
@@ -257,6 +259,54 @@
   </si>
   <si>
     <t>totalprice</t>
+  </si>
+  <si>
+    <t>harpreet</t>
+  </si>
+  <si>
+    <t>harpreet.automation@gmail.com</t>
+  </si>
+  <si>
+    <t>harpreet@123</t>
+  </si>
+  <si>
+    <t>siya</t>
+  </si>
+  <si>
+    <t>siya.automation@gmail.com</t>
+  </si>
+  <si>
+    <t>siya@123</t>
+  </si>
+  <si>
+    <t>kriya</t>
+  </si>
+  <si>
+    <t>kriya.automation@gmail.com</t>
+  </si>
+  <si>
+    <t>kriya@123</t>
+  </si>
+  <si>
+    <t>siyaa</t>
+  </si>
+  <si>
+    <t>siyaa.automation@gmail.com</t>
+  </si>
+  <si>
+    <t>siyaa@123</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>tester1234</t>
+  </si>
+  <si>
+    <t>tester@1234</t>
+  </si>
+  <si>
+    <t>uiautomation123456@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -325,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -352,6 +402,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -666,99 +717,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34817204-1E43-484F-80EF-AB3020F1020E}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{BFB52D7E-0C98-4127-A184-C49B6071E729}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{113CC18B-B582-4D1D-A2D4-7F26840C42C1}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{379AD60A-950D-480F-9015-E697F7896F14}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85730DF-4014-40A2-94CE-5057EDE2CE9D}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -834,7 +792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC0A407-A0FA-40EA-8010-81AAE33F0806}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -989,7 +947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C5766E4-4E0D-48BF-A410-D7112BA2BAA8}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1075,11 +1033,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F5E8E1-C2B7-482F-A21D-FA5B73A9AC84}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1138,4 +1096,272 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34817204-1E43-484F-80EF-AB3020F1020E}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BFB52D7E-0C98-4127-A184-C49B6071E729}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{113CC18B-B582-4D1D-A2D4-7F26840C42C1}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{379AD60A-950D-480F-9015-E697F7896F14}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B57983-1559-4BBB-9757-1C4E09FBCA9D}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{289C7DC4-E6FC-4F5E-9A8F-7B02646812D8}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{D6BC58A8-061B-43AF-91FB-EDB2BDEFEDDD}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{8C60D78E-4DC7-483E-BE8E-BC66A651D675}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{38D83427-7BAB-4F44-926A-8FFBBCCA7BA0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2150847C-796F-4DD1-AE1B-B255AC4DA150}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{26BFCD09-5F01-463D-9680-478527CFFC07}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{D743319C-AA33-4AFA-A304-E4B869A2DA2A}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{B0B9411A-3271-4C69-BA74-8A8DBD10AE49}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{94D8EDA9-0AEF-438A-B381-BC7060C58199}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{F8997E88-C52C-4262-B4C0-486427CDF11F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added selenium grid code
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdatainfo.xlsx
+++ b/src/test/resources/testdata/testdatainfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashwi\eclipse-workspace\AutomationFrameworkOpenCart\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC684228-51A4-4FB7-931B-9C1A988D0A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2454D5-9FC8-48C0-938B-F6296104CF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{B8B23BD0-2100-492A-ADF4-82F66140FD90}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
   <si>
     <t>firstname</t>
   </si>
@@ -306,19 +306,16 @@
     <t>$4,000.00</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>harpreet.automation3@gmail.com</t>
-  </si>
-  <si>
-    <t>siya.automation3@gmail.com</t>
-  </si>
-  <si>
-    <t>kriya.automation3@gmail.com</t>
-  </si>
-  <si>
-    <t>siyaa.automation3@gmail.com</t>
+    <t>harpreet.automation4@gmail.com</t>
+  </si>
+  <si>
+    <t>siya.automation4@gmail.com</t>
+  </si>
+  <si>
+    <t>kriya.automation4@gmail.com</t>
+  </si>
+  <si>
+    <t>siyaa.automation4@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1048,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F5E8E1-C2B7-482F-A21D-FA5B73A9AC84}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A3" sqref="A3:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1059,7 +1056,7 @@
     <col min="6" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
@@ -1082,7 +1079,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1103,11 +1100,6 @@
       </c>
       <c r="G2" s="13" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H7" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1225,8 +1217,8 @@
       <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>89</v>
+      <c r="C1" s="15" t="s">
+        <v>88</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>13</v>
@@ -1246,7 +1238,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>13</v>
@@ -1266,7 +1258,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>13</v>
@@ -1286,7 +1278,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -1304,7 +1296,7 @@
     <hyperlink ref="C4" r:id="rId2" display="siyaa.automation1@gmail.com" xr:uid="{38D83427-7BAB-4F44-926A-8FFBBCCA7BA0}"/>
     <hyperlink ref="C3" r:id="rId3" display="kriya.automation1@gmail.com" xr:uid="{8C60D78E-4DC7-483E-BE8E-BC66A651D675}"/>
     <hyperlink ref="C2" r:id="rId4" display="siya.automation1@gmail.com" xr:uid="{D6BC58A8-061B-43AF-91FB-EDB2BDEFEDDD}"/>
-    <hyperlink ref="C1" r:id="rId5" display="harpreet.automation1@gmail.com" xr:uid="{289C7DC4-E6FC-4F5E-9A8F-7B02646812D8}"/>
+    <hyperlink ref="C1" r:id="rId5" xr:uid="{289C7DC4-E6FC-4F5E-9A8F-7B02646812D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>